<commit_message>
adicionado arquivos de 35 a 39%
</commit_message>
<xml_diff>
--- a/Resultados/INTER_LINEAR/Graficos-1-10 linear.xlsx
+++ b/Resultados/INTER_LINEAR/Graficos-1-10 linear.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukka\Documents\GitHub\OpenCV_Rasp\Resultados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\OpenCV_Rasp\Resultados\INTER_LINEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -120,7 +120,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -234,12 +234,134 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="35"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>21</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>23</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="24">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:pt idx="25">
+                <c:v>26</c:v>
+              </c:pt>
+              <c:pt idx="26">
+                <c:v>27</c:v>
+              </c:pt>
+              <c:pt idx="27">
+                <c:v>28</c:v>
+              </c:pt>
+              <c:pt idx="28">
+                <c:v>29</c:v>
+              </c:pt>
+              <c:pt idx="29">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="30">
+                <c:v>31</c:v>
+              </c:pt>
+              <c:pt idx="31">
+                <c:v>32</c:v>
+              </c:pt>
+              <c:pt idx="32">
+                <c:v>33</c:v>
+              </c:pt>
+              <c:pt idx="33">
+                <c:v>34</c:v>
+              </c:pt>
+              <c:pt idx="34">
+                <c:v>35</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$30:$CW$30</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Plan1!$B$30:$CW$30</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Plan1!$B$30:$AJ$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>234.92</c:v>
                 </c:pt>
@@ -344,201 +466,6 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>268.98</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>272.12</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>270.3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>271.64</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>270.88</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1419.18</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>272.2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>274.44</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>281.60000000000002</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>272.18</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>277.5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>274.94</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>271.7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>271.36</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1441.92</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>277.14</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>272.83999999999997</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>278.45999999999998</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>278.42</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>271.62</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>277.74</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>278.72000000000003</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>277.74</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1450.22</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>275.36</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>275.08</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>276.60000000000002</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>282.10000000000002</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>279.45999999999998</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>276.26</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>277.89999999999998</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>278.56</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>281.45999999999998</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1454.96</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>277.64</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>278.56</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>278.56</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>281.66000000000003</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>278.74</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>278.38</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>279.92</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>280.89999999999998</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>281.38</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1454.8</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>277.86</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>281.52</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>279.42</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>281.16000000000003</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>281.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>279.14</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>279.64</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>276.82</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>278.33999999999997</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1463.32</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>272.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>283.44</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>283.2</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>277.62</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>281.76</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>277.14</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>282.52</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>276.83999999999997</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>277.89999999999998</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>1455.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,8 +481,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-626924688"/>
-        <c:axId val="-626924144"/>
+        <c:axId val="88787824"/>
+        <c:axId val="88776944"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -595,14 +522,17 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$22:$CW$22</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$22:$CW$22</c15:sqref>
+                          <c15:sqref>Plan1!$B$22:$AJ$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -646,14 +576,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$23:$CW$23</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$23:$CW$23</c15:sqref>
+                          <c15:sqref>Plan1!$B$23:$AJ$23</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>51.1</c:v>
                       </c:pt>
@@ -758,201 +691,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>65.94</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>67.900000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>67.2</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>68.319999999999993</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>66.36</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>357.42</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>66.64</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>69.44</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>70.7</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>67.48</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>69.58</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>66.92</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>67.34</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>69.44</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>365.26</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>67.34</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>66.08</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>71.540000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>68.319999999999993</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>67.62</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>69.72</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>69.3</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>66.64</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>361.9</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>68.459999999999994</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>68.739999999999995</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>70.7</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>71.400000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>68.88</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>71.260000000000005</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>68.319999999999993</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>71.540000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>70.98</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>369.32</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>66.78</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>70.14</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>69.72</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>69.16</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>69.16</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>70.84</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>71.680000000000007</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>69.02</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>70.14</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>363.3</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>68.88</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>71.680000000000007</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>72.52</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>74.48</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>71.12</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>70.98</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>70.7</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>68.040000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>70.28</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>370.58</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>66.5</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>73.78</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>72.94</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>69.16</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>71.540000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>70.7</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>72.38</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>71.260000000000005</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>69.58</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>371.42</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -997,14 +735,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$24:$CW$24</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$24:$CW$24</c15:sqref>
+                          <c15:sqref>Plan1!$B$24:$AJ$24</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>54.48</c:v>
                       </c:pt>
@@ -1109,201 +850,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>59.76</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>60.36</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>59.76</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>62.52</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>61.92</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>320.64</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>61.2</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>62.4</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>65.040000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>60.24</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>62.64</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>62.4</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>61.44</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>59.64</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>323.64</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>63.84</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>63.36</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>61.68</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>62.28</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>61.8</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>62.64</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>64.2</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>64.8</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>333</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>63.84</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>62.4</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>61.56</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>64.08</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>63.24</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>62.52</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>65.040000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>63.72</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>62.88</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>330.48</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>66</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>61.56</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>65.400000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>66</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>64.319999999999993</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>64.44</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>65.400000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>65.28</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>65.28</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>332.28</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>63.72</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>64.08</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>62.4</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>63.84</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>65.16</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>62.76</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>64.44</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>64.2</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>63.12</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>332.88</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>63.6</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>62.76</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>63.12</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>64.2</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>63.96</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>62.76</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>65.760000000000005</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>63.24</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>64.92</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>331.8</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1348,14 +894,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$25:$CW$25</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$25:$CW$25</c15:sqref>
+                          <c15:sqref>Plan1!$B$25:$AJ$25</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>40.1</c:v>
                       </c:pt>
@@ -1460,201 +1009,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>39.700000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>43.9</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>41.8</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>40.700000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>41</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>229.4</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>42.2</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>41.3</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>41.8</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>43.4</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>42.3</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>44.4</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>41.1</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>39.799999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>232.6</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>45.7</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>41</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>44</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>44.1</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>42.1</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>42.6</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>43</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>236.9</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>42.9</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>43.1</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>43</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>45.6</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>43.8</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>42.1</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>44.8</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>237.9</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>44.2</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>44.7</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>40.299999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>44.2</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>42.3</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>41.3</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>42.9</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>45.3</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>43.1</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>240.5</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>42.5</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>44.8</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>41.6</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>42.1</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>44.1</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>43.1</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>44.6</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>43.1</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>43.6</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>234.2</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>40.700000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>43.4</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>43.8</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>42.7</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>44.2</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>41.9</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>42.6</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>40.9</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>41.7</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>237</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1699,14 +1053,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$26:$CW$26</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$26:$CW$26</c15:sqref>
+                          <c15:sqref>Plan1!$B$26:$AJ$26</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>38.64</c:v>
                       </c:pt>
@@ -1811,201 +1168,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>43.36</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>40.4</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>41.84</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>41.28</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>42.16</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>212.88</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>43.04</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>42.08</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>43.28</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>42.64</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>42.08</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>42.64</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>42.8</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>215.76</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>41.12</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>41.44</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>41.6</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>43.28</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>41.04</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>42.56</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>42</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>43.36</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>213.6</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>41.28</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>42.56</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>42.08</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>43.36</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>41.6</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>40.799999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>40.72</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>41.92</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>41.28</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>213.44</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>40.880000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>41.36</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>42.24</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>42.4</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>40.96</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>41.68</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>42.16</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>211.12</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>42.08</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>40.96</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>42.48</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>40.479999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>41.6</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>42.8</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>40.880000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>41.52</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>41.04</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>216.32</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>41.2</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>42.08</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>42.08</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>41.84</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>42</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>41.6</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>41.04</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>41.44</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>42.32</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>209.44</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2050,14 +1212,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$27:$CW$27</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$27:$CW$27</c15:sqref>
+                          <c15:sqref>Plan1!$B$27:$AJ$27</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>34.020000000000003</c:v>
                       </c:pt>
@@ -2162,201 +1327,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>34.380000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>34.56</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>34.020000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>33.24</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>33.659999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>169.44</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>33.42</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>33.119999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>34.74</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>33.24</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>34.5</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>33.6</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>34.08</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>34.14</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>171.96</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>32.520000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>34.979999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>33.78</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>34.619999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>32.82</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>34.44</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>34.619999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>34.200000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>172.5</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>33.119999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>32.880000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>32.880000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>33.9</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>33.6</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>33.96</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>33.72</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>33.479999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>34.86</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>168.36</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>33.6</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>34.26</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>34.32</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>33.18</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>34.14</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>33.659999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>33</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>33.54</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>34.5</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>170.4</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>33.72</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>33.119999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>34.32</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>33.9</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>33.18</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>33.42</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>32.64</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>33.72</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>34.26</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>171.36</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>34.020000000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>33.9</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>33.6</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>33.36</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>33.54</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>33.54</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>33</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>33.06</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>33.119999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>169.74</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2403,14 +1373,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$28:$CW$28</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$28:$CW$28</c15:sqref>
+                          <c15:sqref>Plan1!$B$28:$AJ$28</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>9.9600000000000009</c:v>
                       </c:pt>
@@ -2515,201 +1488,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>16.36</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>15.92</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>16.440000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>16.32</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>16.68</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>84.32</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>16.239999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>16.96</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>16.760000000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>16.440000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>16.440000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>16.8</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>16.399999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>86.8</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>17.079999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>16.88</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>16.32</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>16.68</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>17.239999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>16.04</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>16.760000000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>16.64</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>86.92</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>16.52</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>16.72</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>16.72</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>16.96</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>17.32</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>16.52</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>17.399999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>16.760000000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>17.440000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>89.24</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>17.239999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>16.399999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>18.28</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>17.68</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>16.52</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>16.8</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>16.8</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>91.28</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>17.8</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>17.84</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>16.96</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>17.32</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>16.920000000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>17.079999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>16.920000000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>17.16</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>17.04</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>92.6</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>17.079999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>18.16</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>18.48</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>17.079999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>17.440000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>17.559999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>18.48</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>17.64</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>17.2</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>89.68</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2756,14 +1534,17 @@
                   <c:numRef>
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Plan1!$B$29:$CW$29</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Plan1!$B$29:$CW$29</c15:sqref>
+                          <c15:sqref>Plan1!$B$29:$AJ$29</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="100"/>
+                      <c:ptCount val="35"/>
                       <c:pt idx="0">
                         <c:v>6.62</c:v>
                       </c:pt>
@@ -2868,201 +1649,6 @@
                       </c:pt>
                       <c:pt idx="34">
                         <c:v>9.48</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>9.08</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>9.24</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>9.26</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>9.1</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>45.08</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>9.4600000000000009</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>9.14</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>9.2799999999999994</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>8.98</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>9.4</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>8.74</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>9.1</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>9.14</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>45.9</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>9.5399999999999991</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>9.1</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>9.5399999999999991</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>9.14</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>9.74</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>9.44</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>9.1</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>45.4</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>9.24</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>9.3800000000000008</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>9.56</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>9.4</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>9.2200000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>8.8000000000000007</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>8.9</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>9.0399999999999991</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>9.2200000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>46.22</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>8.94</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>9.1</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>9.18</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>9.1999999999999993</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>9.42</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>9.2200000000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>8.98</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>9.2799999999999994</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>9.4</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>45.92</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>9.16</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>9.0399999999999991</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>9.14</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>9.0399999999999991</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>9.32</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>9.4600000000000009</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>9.08</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>45.38</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>9.3000000000000007</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>9.36</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>9.18</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>9.2799999999999994</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>9.08</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>9.08</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>9.26</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>9.3000000000000007</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>9.06</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>46.12</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3074,7 +1660,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-626924688"/>
+        <c:axId val="88787824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3116,7 +1702,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-626924144"/>
+        <c:crossAx val="88776944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3124,7 +1710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-626924144"/>
+        <c:axId val="88776944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +1761,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-626924688"/>
+        <c:crossAx val="88787824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3227,7 +1813,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3270,7 +1856,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3654,8 +2239,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-626919792"/>
-        <c:axId val="-626913808"/>
+        <c:axId val="88791088"/>
+        <c:axId val="88783472"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -6174,7 +4759,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-626919792"/>
+        <c:axId val="88791088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6216,7 +4801,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-626913808"/>
+        <c:crossAx val="88783472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6224,7 +4809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-626913808"/>
+        <c:axId val="88783472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6275,7 +4860,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-626919792"/>
+        <c:crossAx val="88791088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6327,7 +4912,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6748,8 +5333,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-626912720"/>
-        <c:axId val="-626920336"/>
+        <c:axId val="88784560"/>
+        <c:axId val="88777488"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9268,7 +7853,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-626912720"/>
+        <c:axId val="88784560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9311,7 +7896,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-626920336"/>
+        <c:crossAx val="88777488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9319,7 +7904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-626920336"/>
+        <c:axId val="88777488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9370,7 +7955,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-626912720"/>
+        <c:crossAx val="88784560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11199,9 +9784,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -11239,7 +9824,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -11311,7 +9896,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>

</xml_diff>